<commit_message>
Added Testcases for study participation MGT and OSA01 and NCATS Multifilter combinations
</commit_message>
<xml_diff>
--- a/InputFiles/TC60_Canine_Study_OSA01_StudyParticipation_SingleStudy.xlsx
+++ b/InputFiles/TC60_Canine_Study_OSA01_StudyParticipation_SingleStudy.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\sofia0302\Commons_Automation\InputFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\davids3\newclone\sofia0324\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E85C395-5EEA-44C9-A1CD-78E723CA06A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A427355-2209-47A0-B5B1-225F2C5F7E8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -569,8 +569,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C538400-E87C-4027-A918-A51DB80B3430}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" x14ac:dyDescent="0.3"/>

</xml_diff>